<commit_message>
feat(interrupts) Existing functionality retested
</commit_message>
<xml_diff>
--- a/programs/pipelining/structuralhazardloadinstructionswithwriteback.xlsx
+++ b/programs/pipelining/structuralhazardloadinstructionswithwriteback.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\Issie Projects\UART\central-processing-unit\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88327CA9-187B-44A1-875F-8FA19CF460BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8685CD9D-8F06-4BDB-90FD-5EF8BC0D622D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="4950" yWindow="3750" windowWidth="14400" windowHeight="7460" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -264,10 +264,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,12 +588,12 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C1">
         <v>15</v>
       </c>
@@ -643,79 +643,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6" t="s">
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6" t="s">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="6"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -731,10 +731,10 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
@@ -747,76 +747,76 @@
       <c r="L4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6" t="s">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -897,7 +897,7 @@
         <v>C200</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -957,7 +957,7 @@
         <v>7C4</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>E44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>A48</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1156,10 +1156,10 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1178,51 +1178,61 @@
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="S16" s="2"/>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S17" s="2"/>
     </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S18" s="2"/>
     </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S21" s="2"/>
     </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S23" s="2"/>
     </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C24" s="4"/>
       <c r="S24" s="2"/>
     </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S25" s="2"/>
     </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S26" s="2"/>
     </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S27" s="2"/>
     </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="S29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="K6:P6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="K2:M2"/>
@@ -1232,16 +1242,6 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1253,43 +1253,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8303367F-86F1-47C6-AF22-70C59577B968}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
       <c r="D2">
         <v>0</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1428,20 +1428,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C9" s="6" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D10">
         <v>0</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>46</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>48</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>49</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
@@ -1567,7 +1567,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>53</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>54</v>
       </c>

</xml_diff>